<commit_message>
update the third release plan with actual time
</commit_message>
<xml_diff>
--- a/PMP/ReleasePlanning_thirdRelease_FoodiesWebApp_v1.xlsx
+++ b/PMP/ReleasePlanning_thirdRelease_FoodiesWebApp_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df7bb8cccf9c71e3/Dokumenter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sagedwael/Documents/GitHub/QA-Workshop_Foodies/PMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8928A64E-AB38-4935-AC8C-59F6F7A71055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FAE54B-2F91-DC4F-9B51-CB11BE4D502F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{E9C65AA8-DBCD-8542-AAC2-582E5FCA2851}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17380" xr2:uid="{E9C65AA8-DBCD-8542-AAC2-582E5FCA2851}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -205,7 +205,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -692,18 +692,18 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.625" customWidth="1"/>
-    <col min="2" max="2" width="26.375" customWidth="1"/>
-    <col min="3" max="3" width="34.375" customWidth="1"/>
-    <col min="4" max="4" width="19.625" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -722,7 +722,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
@@ -741,7 +741,7 @@
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="19"/>
       <c r="B3" s="19"/>
       <c r="C3" s="2" t="s">
@@ -756,7 +756,7 @@
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="19"/>
       <c r="B4" s="19"/>
       <c r="C4" s="2" t="s">
@@ -771,7 +771,7 @@
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="19"/>
       <c r="B5" s="19"/>
       <c r="C5" s="2" t="s">
@@ -786,7 +786,7 @@
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="19"/>
       <c r="C6" s="2" t="s">
@@ -801,7 +801,7 @@
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="2" t="s">
@@ -816,7 +816,7 @@
       <c r="F7" s="11"/>
       <c r="G7" s="11"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="19"/>
       <c r="C8" s="2" t="s">
@@ -831,7 +831,7 @@
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="19"/>
       <c r="B9" s="19"/>
       <c r="C9" s="2"/>
@@ -840,7 +840,7 @@
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
         <v>21</v>
       </c>
@@ -859,7 +859,7 @@
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="20"/>
       <c r="B11" s="21"/>
       <c r="C11" s="3" t="s">
@@ -874,7 +874,7 @@
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="20"/>
       <c r="B12" s="21"/>
       <c r="C12" s="3" t="s">
@@ -889,7 +889,7 @@
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="20"/>
       <c r="B13" s="21"/>
       <c r="C13" s="3" t="s">
@@ -904,7 +904,7 @@
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="20"/>
       <c r="B14" s="21"/>
       <c r="C14" s="3" t="s">
@@ -919,7 +919,7 @@
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="20"/>
       <c r="B15" s="21"/>
       <c r="C15" s="3" t="s">
@@ -934,7 +934,7 @@
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="20"/>
       <c r="B16" s="21"/>
       <c r="C16" s="3" t="s">
@@ -949,7 +949,7 @@
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>30</v>
       </c>
@@ -968,7 +968,7 @@
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
     </row>
-    <row r="18" spans="1:7" ht="21" customHeight="1">
+    <row r="18" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="17"/>
       <c r="B18" s="17"/>
       <c r="C18" s="4" t="s">
@@ -983,7 +983,7 @@
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
     </row>
-    <row r="19" spans="1:7" ht="26.1" customHeight="1">
+    <row r="19" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="17"/>
       <c r="B19" s="17"/>
       <c r="C19" s="4" t="s">
@@ -998,7 +998,7 @@
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
     </row>
-    <row r="20" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
         <v>35</v>
       </c>
@@ -1017,7 +1017,7 @@
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
       <c r="B21" s="18"/>
       <c r="C21" s="9" t="s">
@@ -1032,7 +1032,7 @@
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="18"/>
       <c r="B22" s="18"/>
       <c r="C22" s="9" t="s">
@@ -1047,7 +1047,7 @@
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="9" t="s">
@@ -1062,7 +1062,7 @@
       <c r="F23" s="12"/>
       <c r="G23" s="12"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="18"/>
       <c r="B24" s="18"/>
       <c r="C24" s="9" t="s">
@@ -1077,7 +1077,7 @@
       <c r="F24" s="12"/>
       <c r="G24" s="12"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="18"/>
       <c r="B25" s="18"/>
       <c r="C25" s="9" t="s">
@@ -1092,7 +1092,7 @@
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
       <c r="C26" s="9" t="s">
@@ -1107,7 +1107,7 @@
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>44</v>
       </c>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="F28" s="14"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>49</v>
       </c>
@@ -1139,10 +1139,12 @@
       <c r="D29" s="5">
         <v>4</v>
       </c>
-      <c r="E29" s="5"/>
+      <c r="E29" s="5">
+        <v>14</v>
+      </c>
       <c r="F29" s="15"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>16</v>
       </c>
@@ -1156,10 +1158,12 @@
       <c r="D30" s="5">
         <v>1</v>
       </c>
-      <c r="E30" s="5"/>
+      <c r="E30" s="5">
+        <v>11</v>
+      </c>
       <c r="F30" s="15"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>50</v>
       </c>
@@ -1173,10 +1177,12 @@
       <c r="D31" s="5">
         <v>0</v>
       </c>
-      <c r="E31" s="5"/>
+      <c r="E31" s="5">
+        <v>10</v>
+      </c>
       <c r="F31" s="15"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>10</v>
       </c>
@@ -1190,10 +1196,12 @@
       <c r="D32" s="5">
         <v>2.5</v>
       </c>
-      <c r="E32" s="5"/>
+      <c r="E32" s="5">
+        <v>11</v>
+      </c>
       <c r="F32" s="15"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>51</v>
       </c>
@@ -1207,10 +1215,12 @@
       <c r="D33" s="5">
         <v>1</v>
       </c>
-      <c r="E33" s="5"/>
+      <c r="E33" s="5">
+        <v>9</v>
+      </c>
       <c r="F33" s="15"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>52</v>
       </c>
@@ -1224,10 +1234,12 @@
       <c r="D34" s="5">
         <v>1</v>
       </c>
-      <c r="E34" s="5"/>
+      <c r="E34" s="5">
+        <v>11</v>
+      </c>
       <c r="F34" s="15"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>53</v>
       </c>
@@ -1245,11 +1257,11 @@
       </c>
       <c r="E35" s="5">
         <f>SUM(E29:E34)</f>
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="F35" s="15"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>

</xml_diff>